<commit_message>
text:Segunda parte pruebas funcionales crear modelo
</commit_message>
<xml_diff>
--- a/docs/User Test/Plan de Pruebas Funcionales antes de la Release.xlsx
+++ b/docs/User Test/Plan de Pruebas Funcionales antes de la Release.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdel\Documents\ING SOFTWARE\PROYECTO GRUPOS\TRABAJO-ENX\docs\User Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98028CD1-4332-453B-89C0-FE33622FCA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8884AAC4-E359-4542-AF91-5B80B637F4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{02A0193E-1715-4B71-95BD-40B54D444483}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -201,6 +201,138 @@
   </si>
   <si>
     <t>Ventana de Bienvenida y se carga el programa</t>
+  </si>
+  <si>
+    <t>CrM13</t>
+  </si>
+  <si>
+    <t>1-Se selecciona Eliminar filas y se aplica</t>
+  </si>
+  <si>
+    <t>CrM14</t>
+  </si>
+  <si>
+    <t>1-Se selecciona Rellenar con Media y se Aplica</t>
+  </si>
+  <si>
+    <t>CrM15</t>
+  </si>
+  <si>
+    <t>1-Se selecciona Rellenar con Mediana y se Aplica</t>
+  </si>
+  <si>
+    <t>CrM16</t>
+  </si>
+  <si>
+    <t>1-Se selecciona Rellenar con Constante y se Aplica</t>
+  </si>
+  <si>
+    <t>Notificación Error de Validación</t>
+  </si>
+  <si>
+    <t>CrM17</t>
+  </si>
+  <si>
+    <t>1-Se selecciona Rellenar con Constante, se escribe una constante y Aplica</t>
+  </si>
+  <si>
+    <t>CrM18</t>
+  </si>
+  <si>
+    <t>Separación de Datos</t>
+  </si>
+  <si>
+    <t>CrM15||13||14||17||8</t>
+  </si>
+  <si>
+    <t>Nueva sección División de Datos</t>
+  </si>
+  <si>
+    <t>CrM19</t>
+  </si>
+  <si>
+    <t>1-Se escoge un valor no numérico de Semilla y se Divide</t>
+  </si>
+  <si>
+    <t>Notificación de Error</t>
+  </si>
+  <si>
+    <t>CrM20</t>
+  </si>
+  <si>
+    <t>1- No se escoge un valor entre 0 y 10000000000 y se Divide</t>
+  </si>
+  <si>
+    <t>❌</t>
+  </si>
+  <si>
+    <t>CrM21</t>
+  </si>
+  <si>
+    <t>1-Se escoge un valor entre 0 y 10000000000 y se Divide</t>
+  </si>
+  <si>
+    <t>CrM22</t>
+  </si>
+  <si>
+    <t>1-Se comprueban la funcionalidad del slider y se Divide</t>
+  </si>
+  <si>
+    <t>CrM23</t>
+  </si>
+  <si>
+    <t>Crear Modelo</t>
+  </si>
+  <si>
+    <t>CrM21||CrM22</t>
+  </si>
+  <si>
+    <t>Nueva sección Visualización dle Modelo</t>
+  </si>
+  <si>
+    <t>CrM24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CrM23 &amp;&amp; CrM8 </t>
+  </si>
+  <si>
+    <t>1-Se acepta la notificación de más de una variable de entrada</t>
+  </si>
+  <si>
+    <t>CrM25</t>
+  </si>
+  <si>
+    <t>CrM23 ||CrM24</t>
+  </si>
+  <si>
+    <t>1-Se comprueba la fórmula con los nombres de las columnas seleccionadas</t>
+  </si>
+  <si>
+    <t>Presentación correcta de la fórmula</t>
+  </si>
+  <si>
+    <t>CrM26</t>
+  </si>
+  <si>
+    <t>CrM23||CrM24</t>
+  </si>
+  <si>
+    <t>1-Se comprueba R 2 y el EMC de entrenamiento y test</t>
+  </si>
+  <si>
+    <t>Valores correctamente calculados</t>
+  </si>
+  <si>
+    <t>CrM27</t>
+  </si>
+  <si>
+    <t>(CrM23||CrM24)&amp;&amp;CrM10</t>
+  </si>
+  <si>
+    <t>1-Se comprueban ambas gráficas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Representación correccta </t>
   </si>
 </sst>
 </file>
@@ -295,8 +427,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C865C549-F8D7-491B-B5A0-DEAEC76F60E7}" name="Tabla1" displayName="Tabla1" ref="D1:I15" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="D1:I15" xr:uid="{C865C549-F8D7-491B-B5A0-DEAEC76F60E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C865C549-F8D7-491B-B5A0-DEAEC76F60E7}" name="Tabla1" displayName="Tabla1" ref="D1:I30" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="D1:I30" xr:uid="{C865C549-F8D7-491B-B5A0-DEAEC76F60E7}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{89E5CABB-DA9A-41F4-819F-F69C7B220B9A}" name="ID"/>
     <tableColumn id="2" xr3:uid="{C0F89E4A-52E1-4F79-8B03-593ECF0BF318}" name="FUNCIONALIDAD"/>
@@ -629,7 +761,7 @@
   <dimension ref="C1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="118" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,6 +1067,306 @@
         <v>9</v>
       </c>
     </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" t="s">
+        <v>83</v>
+      </c>
+      <c r="I26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" t="s">
+        <v>93</v>
+      </c>
+      <c r="H29" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G38" s="2"/>
     </row>

</xml_diff>

<commit_message>
test:Final de Crea Modelo y prinipio de Carga, pruebas funcionales
</commit_message>
<xml_diff>
--- a/docs/User Test/Plan de Pruebas Funcionales antes de la Release.xlsx
+++ b/docs/User Test/Plan de Pruebas Funcionales antes de la Release.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdel\Documents\ING SOFTWARE\PROYECTO GRUPOS\TRABAJO-ENX\docs\User Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8884AAC4-E359-4542-AF91-5B80B637F4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EE6FFC-42F9-434C-B4FD-10A8AEFBE4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{02A0193E-1715-4B71-95BD-40B54D444483}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="148">
   <si>
     <t>ID</t>
   </si>
@@ -333,6 +333,153 @@
   </si>
   <si>
     <t xml:space="preserve">Representación correccta </t>
+  </si>
+  <si>
+    <t>CrM28</t>
+  </si>
+  <si>
+    <t>1-Se prueba a redactar una descripción del modelo</t>
+  </si>
+  <si>
+    <t>La descripción se muestra correctamente</t>
+  </si>
+  <si>
+    <t>CrM29</t>
+  </si>
+  <si>
+    <t>Guardar Modelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Se presiona el botón "Guardar Modelo" </t>
+  </si>
+  <si>
+    <t>Ventana Emergete para seleccionar carpeta</t>
+  </si>
+  <si>
+    <t>CrM30</t>
+  </si>
+  <si>
+    <t>1-Se selecciona una carpeta sin permisos (Ejemplo: System32)</t>
+  </si>
+  <si>
+    <t>Notificación de Error "Permission denied"</t>
+  </si>
+  <si>
+    <t>CrM31</t>
+  </si>
+  <si>
+    <t>1-Se selecciona un disco sin espacio suficiente</t>
+  </si>
+  <si>
+    <t>Notifcación de Error</t>
+  </si>
+  <si>
+    <t>❓</t>
+  </si>
+  <si>
+    <t>CrM32</t>
+  </si>
+  <si>
+    <t>1-Se selecciona una carpeta válida</t>
+  </si>
+  <si>
+    <t>CrM33</t>
+  </si>
+  <si>
+    <t>Se Guarda el modelo/descripción</t>
+  </si>
+  <si>
+    <t>CrM34</t>
+  </si>
+  <si>
+    <t>Predicción del Modelo</t>
+  </si>
+  <si>
+    <t>CrM33||CrM23||CrM24</t>
+  </si>
+  <si>
+    <t>1-Se comprueba el panel "Predicción con modelo"</t>
+  </si>
+  <si>
+    <t>Panel correcto para la predicción</t>
+  </si>
+  <si>
+    <t>CrM35</t>
+  </si>
+  <si>
+    <t>1-Se comprueba que la entrada/salida son las respectivas columnas seleccionadas</t>
+  </si>
+  <si>
+    <t>Panel dividido correctamente</t>
+  </si>
+  <si>
+    <t>CrM36</t>
+  </si>
+  <si>
+    <t>1-No se escribe una entrada o se escribe un valor no numérico y se predice</t>
+  </si>
+  <si>
+    <t>Notificación de Error "Valores no numéricos"</t>
+  </si>
+  <si>
+    <t>CrM37</t>
+  </si>
+  <si>
+    <t>1-Se escribe un valor numérico en la entrada y se predice</t>
+  </si>
+  <si>
+    <t>Se predice correctamente la salida</t>
+  </si>
+  <si>
+    <t>CrM38</t>
+  </si>
+  <si>
+    <t>CrM(1||2||…..||37)</t>
+  </si>
+  <si>
+    <t>1-Se carga otro archivo</t>
+  </si>
+  <si>
+    <t>Se reinician todos los paneles</t>
+  </si>
+  <si>
+    <t>CaM0</t>
+  </si>
+  <si>
+    <t>Cargar Modelo</t>
+  </si>
+  <si>
+    <t>1-Se presiona el botón "Cargar Modelo" arriba a la izquierda</t>
+  </si>
+  <si>
+    <t>Nueva pestaña con paneles para cargar modelo</t>
+  </si>
+  <si>
+    <t>CaM1</t>
+  </si>
+  <si>
+    <t>1-Se presiona el botón"Cargar Modelo" del panel "Cargar Modelo Guardado"</t>
+  </si>
+  <si>
+    <t>Nueva ventana para selección de archivo</t>
+  </si>
+  <si>
+    <t>CaM2</t>
+  </si>
+  <si>
+    <t>1-Se exploran archivos</t>
+  </si>
+  <si>
+    <t>Solo se aceptan arhcivos Joblib</t>
+  </si>
+  <si>
+    <t>CaM3</t>
+  </si>
+  <si>
+    <t>1-Se selecciona un archivo corrupto</t>
+  </si>
+  <si>
+    <t>Notificación de Error "Error al cargar el modelo"</t>
   </si>
 </sst>
 </file>
@@ -427,8 +574,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C865C549-F8D7-491B-B5A0-DEAEC76F60E7}" name="Tabla1" displayName="Tabla1" ref="D1:I30" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="D1:I30" xr:uid="{C865C549-F8D7-491B-B5A0-DEAEC76F60E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C865C549-F8D7-491B-B5A0-DEAEC76F60E7}" name="Tabla1" displayName="Tabla1" ref="D1:I46" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="D1:I46" xr:uid="{C865C549-F8D7-491B-B5A0-DEAEC76F60E7}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{89E5CABB-DA9A-41F4-819F-F69C7B220B9A}" name="ID"/>
     <tableColumn id="2" xr3:uid="{C0F89E4A-52E1-4F79-8B03-593ECF0BF318}" name="FUNCIONALIDAD"/>
@@ -760,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480CF6BA-EE37-47B7-9844-60E33DB6B147}">
   <dimension ref="C1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="118" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="118" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,11 +1514,306 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G38" s="2"/>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" t="s">
+        <v>100</v>
+      </c>
+      <c r="H31" t="s">
+        <v>101</v>
+      </c>
+      <c r="I31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" t="s">
+        <v>104</v>
+      </c>
+      <c r="H32" t="s">
+        <v>105</v>
+      </c>
+      <c r="I32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" t="s">
+        <v>103</v>
+      </c>
+      <c r="F33" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" t="s">
+        <v>108</v>
+      </c>
+      <c r="I33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" t="s">
+        <v>103</v>
+      </c>
+      <c r="F34" t="s">
+        <v>102</v>
+      </c>
+      <c r="G34" t="s">
+        <v>110</v>
+      </c>
+      <c r="H34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35" t="s">
+        <v>114</v>
+      </c>
+      <c r="H35" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" t="s">
+        <v>103</v>
+      </c>
+      <c r="F36" t="s">
+        <v>102</v>
+      </c>
+      <c r="G36" t="s">
+        <v>36</v>
+      </c>
+      <c r="H36" t="s">
+        <v>116</v>
+      </c>
+      <c r="I36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" t="s">
+        <v>118</v>
+      </c>
+      <c r="F37" t="s">
+        <v>119</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H37" t="s">
+        <v>121</v>
+      </c>
+      <c r="I37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" t="s">
+        <v>123</v>
+      </c>
+      <c r="H38" t="s">
+        <v>124</v>
+      </c>
+      <c r="I38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" t="s">
+        <v>118</v>
+      </c>
+      <c r="F39" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" t="s">
+        <v>126</v>
+      </c>
+      <c r="H39" t="s">
+        <v>127</v>
+      </c>
+      <c r="I39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" t="s">
+        <v>118</v>
+      </c>
+      <c r="F40" t="s">
+        <v>117</v>
+      </c>
+      <c r="G40" t="s">
+        <v>129</v>
+      </c>
+      <c r="H40" t="s">
+        <v>130</v>
+      </c>
+      <c r="I40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
+      <c r="D41" t="s">
+        <v>131</v>
+      </c>
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" t="s">
+        <v>132</v>
+      </c>
+      <c r="G41" t="s">
+        <v>133</v>
+      </c>
+      <c r="H41" t="s">
+        <v>134</v>
+      </c>
+      <c r="I41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E42" t="s">
+        <v>136</v>
+      </c>
+      <c r="F42" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" t="s">
+        <v>137</v>
+      </c>
+      <c r="H42" t="s">
+        <v>138</v>
+      </c>
+      <c r="I42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" t="s">
+        <v>136</v>
+      </c>
+      <c r="F43" t="s">
+        <v>135</v>
+      </c>
+      <c r="G43" t="s">
+        <v>140</v>
+      </c>
+      <c r="H43" t="s">
+        <v>141</v>
+      </c>
+      <c r="I43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>142</v>
+      </c>
+      <c r="E44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F44" t="s">
+        <v>139</v>
+      </c>
+      <c r="G44" t="s">
+        <v>143</v>
+      </c>
+      <c r="H44" t="s">
+        <v>144</v>
+      </c>
+      <c r="I44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>145</v>
+      </c>
+      <c r="E45" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45" t="s">
+        <v>142</v>
+      </c>
+      <c r="G45" t="s">
+        <v>146</v>
+      </c>
+      <c r="H45" t="s">
+        <v>147</v>
+      </c>
+      <c r="I45" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="51" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G51" s="2"/>

</xml_diff>

<commit_message>
test: Fin pruebas funcionales , Cargar Modelo y Research
</commit_message>
<xml_diff>
--- a/docs/User Test/Plan de Pruebas Funcionales antes de la Release.xlsx
+++ b/docs/User Test/Plan de Pruebas Funcionales antes de la Release.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdel\Documents\ING SOFTWARE\PROYECTO GRUPOS\TRABAJO-ENX\docs\User Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdel\Documents\ING SOFTWARE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EE6FFC-42F9-434C-B4FD-10A8AEFBE4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AE4850-71E2-4D03-9E52-0FB34299528B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{02A0193E-1715-4B71-95BD-40B54D444483}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="195">
   <si>
     <t>ID</t>
   </si>
@@ -71,6 +71,9 @@
     <t>1-Hacer click en el botón "Cargar Datos"</t>
   </si>
   <si>
+    <t>Crear Modelo</t>
+  </si>
+  <si>
     <t>CrM0</t>
   </si>
   <si>
@@ -134,6 +137,9 @@
     <t>CrM7</t>
   </si>
   <si>
+    <t>❌</t>
+  </si>
+  <si>
     <t>CrM8</t>
   </si>
   <si>
@@ -176,15 +182,84 @@
     <t>CrM12</t>
   </si>
   <si>
+    <t>CrM13</t>
+  </si>
+  <si>
+    <t>CrM14</t>
+  </si>
+  <si>
     <t>Barra de carga y Notificación de Éxito</t>
   </si>
   <si>
+    <t>1-Se selecciona Eliminar filas y se aplica</t>
+  </si>
+  <si>
     <t>1-No se elige ninguna opción para el procesado de datos y se Aplica</t>
   </si>
   <si>
+    <t>1-Se selecciona Rellenar con Media y se Aplica</t>
+  </si>
+  <si>
     <t>Notificación de Éxito</t>
   </si>
   <si>
+    <t>CrM15</t>
+  </si>
+  <si>
+    <t>CrM16</t>
+  </si>
+  <si>
+    <t>CrM17</t>
+  </si>
+  <si>
+    <t>CrM18</t>
+  </si>
+  <si>
+    <t>CrM19</t>
+  </si>
+  <si>
+    <t>CrM20</t>
+  </si>
+  <si>
+    <t>CrM21</t>
+  </si>
+  <si>
+    <t>CrM22</t>
+  </si>
+  <si>
+    <t>CrM23</t>
+  </si>
+  <si>
+    <t>1-Se selecciona Rellenar con Mediana y se Aplica</t>
+  </si>
+  <si>
+    <t>1-Se selecciona Rellenar con Constante y se Aplica</t>
+  </si>
+  <si>
+    <t>Notificación Error de Validación</t>
+  </si>
+  <si>
+    <t>1-Se selecciona Rellenar con Constante, se escribe una constante y Aplica</t>
+  </si>
+  <si>
+    <t>Separación de Datos</t>
+  </si>
+  <si>
+    <t>Nueva sección División de Datos</t>
+  </si>
+  <si>
+    <t>Notificación de Error</t>
+  </si>
+  <si>
+    <t>1- No se escoge un valor entre 0 y 10000000000 y se Divide</t>
+  </si>
+  <si>
+    <t>1-Se escoge un valor no numérico de Semilla y se Divide</t>
+  </si>
+  <si>
+    <t>1-Se escoge un valor entre 0 y 10000000000 y se Divide</t>
+  </si>
+  <si>
     <t>1-Se usa scrollbar de la aplicación</t>
   </si>
   <si>
@@ -194,292 +269,358 @@
     <t>1-Se seleccionan columas con nulos (etrada/salida) y se Confirma</t>
   </si>
   <si>
+    <t>1-Se comprueban la funcionalidad del slider y se Divide</t>
+  </si>
+  <si>
+    <t>Nueva sección Visualización dle Modelo</t>
+  </si>
+  <si>
+    <t>1-Se comprueba la fórmula con los nombres de las columnas seleccionadas</t>
+  </si>
+  <si>
+    <t>Presentación correcta de la fórmula</t>
+  </si>
+  <si>
+    <t>CrM24</t>
+  </si>
+  <si>
+    <t>CrM25</t>
+  </si>
+  <si>
+    <t>CrM26</t>
+  </si>
+  <si>
+    <t>CrM27</t>
+  </si>
+  <si>
+    <t>CrM28</t>
+  </si>
+  <si>
+    <t>CrM29</t>
+  </si>
+  <si>
+    <t>CrM30</t>
+  </si>
+  <si>
+    <t>CrM31</t>
+  </si>
+  <si>
+    <t>CrM32</t>
+  </si>
+  <si>
+    <t>CrM33</t>
+  </si>
+  <si>
+    <t>CrM34</t>
+  </si>
+  <si>
+    <t>CrM35</t>
+  </si>
+  <si>
+    <t>CrM36</t>
+  </si>
+  <si>
+    <t>CrM37</t>
+  </si>
+  <si>
+    <t>CrM38</t>
+  </si>
+  <si>
+    <t>1-Se comprueba R 2 y el EMC de entrenamiento y test</t>
+  </si>
+  <si>
+    <t>Valores correctamente calculados</t>
+  </si>
+  <si>
+    <t>CrM15||13||14||17||8</t>
+  </si>
+  <si>
+    <t>CrM21||CrM22</t>
+  </si>
+  <si>
     <t>1-Se selecciona una columna de entrada y salida sin null y se Confirma</t>
   </si>
   <si>
+    <t xml:space="preserve">CrM23 &amp;&amp; CrM8 </t>
+  </si>
+  <si>
+    <t>1-Se acepta la notificación de más de una variable de entrada</t>
+  </si>
+  <si>
+    <t>CrM23 ||CrM24</t>
+  </si>
+  <si>
+    <t>CrM23||CrM24</t>
+  </si>
+  <si>
+    <t>(CrM23||CrM24)&amp;&amp;CrM10</t>
+  </si>
+  <si>
     <t>CrM11||CrM10</t>
   </si>
   <si>
+    <t>1-Se comprueban ambas gráficas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Representación correccta </t>
+  </si>
+  <si>
+    <t>1-Se prueba a redactar una descripción del modelo</t>
+  </si>
+  <si>
+    <t>La descripción se muestra correctamente</t>
+  </si>
+  <si>
+    <t>Guardar Modelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Se presiona el botón "Guardar Modelo" </t>
+  </si>
+  <si>
+    <t>Ventana Emergete para seleccionar carpeta</t>
+  </si>
+  <si>
+    <t>1-Se selecciona una carpeta sin permisos (Ejemplo: System32)</t>
+  </si>
+  <si>
+    <t>1-Se selecciona un disco sin espacio suficiente</t>
+  </si>
+  <si>
+    <t>Notifcación de Error</t>
+  </si>
+  <si>
+    <t>❓</t>
+  </si>
+  <si>
+    <t>Notificación de Error "Permission denied"</t>
+  </si>
+  <si>
+    <t>1-Se selecciona una carpeta válida</t>
+  </si>
+  <si>
+    <t>Se Guarda el modelo/descripción</t>
+  </si>
+  <si>
+    <t>Predicción del Modelo</t>
+  </si>
+  <si>
+    <t>CrM33||CrM23||CrM24</t>
+  </si>
+  <si>
+    <t>1-Se comprueba el panel "Predicción con modelo"</t>
+  </si>
+  <si>
+    <t>Panel correcto para la predicción</t>
+  </si>
+  <si>
+    <t>1-Se comprueba que la entrada/salida son las respectivas columnas seleccionadas</t>
+  </si>
+  <si>
+    <t>Panel dividido correctamente</t>
+  </si>
+  <si>
+    <t>Notificación de Error "Valores no numéricos"</t>
+  </si>
+  <si>
+    <t>1-No se escribe una entrada o se escribe un valor no numérico y se predice</t>
+  </si>
+  <si>
+    <t>1-Se escribe un valor numérico en la entrada y se predice</t>
+  </si>
+  <si>
+    <t>CaM0</t>
+  </si>
+  <si>
+    <t>Cargar Modelo</t>
+  </si>
+  <si>
+    <t>Se predice correctamente la salida</t>
+  </si>
+  <si>
+    <t>1-Se carga otro archivo</t>
+  </si>
+  <si>
+    <t>Se reinician todos los paneles</t>
+  </si>
+  <si>
+    <t>CaM1</t>
+  </si>
+  <si>
+    <t>CaM2</t>
+  </si>
+  <si>
+    <t>CaM3</t>
+  </si>
+  <si>
+    <t>CaM4</t>
+  </si>
+  <si>
+    <t>CaM5</t>
+  </si>
+  <si>
+    <t>CaM6</t>
+  </si>
+  <si>
+    <t>CaM7</t>
+  </si>
+  <si>
+    <t>CaM8</t>
+  </si>
+  <si>
+    <t>CaM9</t>
+  </si>
+  <si>
+    <t>CaM10</t>
+  </si>
+  <si>
+    <t>CaM11</t>
+  </si>
+  <si>
+    <t>CaM12</t>
+  </si>
+  <si>
+    <t>CaM13</t>
+  </si>
+  <si>
+    <t>1-Se presiona el botón "Cargar Modelo" arriba a la izquierda</t>
+  </si>
+  <si>
+    <t>Nueva pestaña con paneles para cargar modelo</t>
+  </si>
+  <si>
+    <t>CrM(1||2||…..||37)</t>
+  </si>
+  <si>
+    <t>1-Se presiona el botón"Cargar Modelo" del panel "Cargar Modelo Guardado"</t>
+  </si>
+  <si>
+    <t>Nueva ventana para selección de archivo</t>
+  </si>
+  <si>
+    <t>1-Se exploran archivos</t>
+  </si>
+  <si>
+    <t>Solo se aceptan arhcivos Joblib</t>
+  </si>
+  <si>
+    <t>1-Se selecciona un archivo corrupto</t>
+  </si>
+  <si>
+    <t>Notificación de Error "Error al cargar el modelo"</t>
+  </si>
+  <si>
+    <t>1-Se selecciona un archivo correcto</t>
+  </si>
+  <si>
+    <t>Notificación de Éxito "Modelo cargado"</t>
+  </si>
+  <si>
+    <t>1-Se acepta o cierra la notificación</t>
+  </si>
+  <si>
+    <t>Paneles Modelo Cargado, Descripción y Predicción</t>
+  </si>
+  <si>
+    <t>Modelo Cargado</t>
+  </si>
+  <si>
+    <t>1-Se comprueba la fórmla cargada, R2, EMC y las columnas salida/entrada</t>
+  </si>
+  <si>
+    <t>Fórmula, R2, EMC y respectivas columnas correcta</t>
+  </si>
+  <si>
+    <t>1-Se comprueba el panel de decripción</t>
+  </si>
+  <si>
+    <t>Carga la respectiva descripción guardada</t>
+  </si>
+  <si>
+    <t>1-Se comprueba que la entrada/salida son las respectivas columnas guardadas</t>
+  </si>
+  <si>
+    <t>Panel creado correctamente para la predicción</t>
+  </si>
+  <si>
+    <t>1-Se carga otro modelo</t>
+  </si>
+  <si>
+    <t>CaM(4||5||…..11)</t>
+  </si>
+  <si>
     <t>Ventana de Bienvenida y se carga el programa</t>
   </si>
   <si>
-    <t>CrM13</t>
-  </si>
-  <si>
-    <t>1-Se selecciona Eliminar filas y se aplica</t>
-  </si>
-  <si>
-    <t>CrM14</t>
-  </si>
-  <si>
-    <t>1-Se selecciona Rellenar con Media y se Aplica</t>
-  </si>
-  <si>
-    <t>CrM15</t>
-  </si>
-  <si>
-    <t>1-Se selecciona Rellenar con Mediana y se Aplica</t>
-  </si>
-  <si>
-    <t>CrM16</t>
-  </si>
-  <si>
-    <t>1-Se selecciona Rellenar con Constante y se Aplica</t>
-  </si>
-  <si>
-    <t>Notificación Error de Validación</t>
-  </si>
-  <si>
-    <t>CrM17</t>
-  </si>
-  <si>
-    <t>1-Se selecciona Rellenar con Constante, se escribe una constante y Aplica</t>
-  </si>
-  <si>
-    <t>CrM18</t>
-  </si>
-  <si>
-    <t>Separación de Datos</t>
-  </si>
-  <si>
-    <t>CrM15||13||14||17||8</t>
-  </si>
-  <si>
-    <t>Nueva sección División de Datos</t>
-  </si>
-  <si>
-    <t>CrM19</t>
-  </si>
-  <si>
-    <t>1-Se escoge un valor no numérico de Semilla y se Divide</t>
-  </si>
-  <si>
-    <t>Notificación de Error</t>
-  </si>
-  <si>
-    <t>CrM20</t>
-  </si>
-  <si>
-    <t>1- No se escoge un valor entre 0 y 10000000000 y se Divide</t>
-  </si>
-  <si>
-    <t>❌</t>
-  </si>
-  <si>
-    <t>CrM21</t>
-  </si>
-  <si>
-    <t>1-Se escoge un valor entre 0 y 10000000000 y se Divide</t>
-  </si>
-  <si>
-    <t>CrM22</t>
-  </si>
-  <si>
-    <t>1-Se comprueban la funcionalidad del slider y se Divide</t>
-  </si>
-  <si>
-    <t>CrM23</t>
-  </si>
-  <si>
-    <t>Crear Modelo</t>
-  </si>
-  <si>
-    <t>CrM21||CrM22</t>
-  </si>
-  <si>
-    <t>Nueva sección Visualización dle Modelo</t>
-  </si>
-  <si>
-    <t>CrM24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CrM23 &amp;&amp; CrM8 </t>
-  </si>
-  <si>
-    <t>1-Se acepta la notificación de más de una variable de entrada</t>
-  </si>
-  <si>
-    <t>CrM25</t>
-  </si>
-  <si>
-    <t>CrM23 ||CrM24</t>
-  </si>
-  <si>
-    <t>1-Se comprueba la fórmula con los nombres de las columnas seleccionadas</t>
-  </si>
-  <si>
-    <t>Presentación correcta de la fórmula</t>
-  </si>
-  <si>
-    <t>CrM26</t>
-  </si>
-  <si>
-    <t>CrM23||CrM24</t>
-  </si>
-  <si>
-    <t>1-Se comprueba R 2 y el EMC de entrenamiento y test</t>
-  </si>
-  <si>
-    <t>Valores correctamente calculados</t>
-  </si>
-  <si>
-    <t>CrM27</t>
-  </si>
-  <si>
-    <t>(CrM23||CrM24)&amp;&amp;CrM10</t>
-  </si>
-  <si>
-    <t>1-Se comprueban ambas gráficas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Representación correccta </t>
-  </si>
-  <si>
-    <t>CrM28</t>
-  </si>
-  <si>
-    <t>1-Se prueba a redactar una descripción del modelo</t>
-  </si>
-  <si>
-    <t>La descripción se muestra correctamente</t>
-  </si>
-  <si>
-    <t>CrM29</t>
-  </si>
-  <si>
-    <t>Guardar Modelo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-Se presiona el botón "Guardar Modelo" </t>
-  </si>
-  <si>
-    <t>Ventana Emergete para seleccionar carpeta</t>
-  </si>
-  <si>
-    <t>CrM30</t>
-  </si>
-  <si>
-    <t>1-Se selecciona una carpeta sin permisos (Ejemplo: System32)</t>
-  </si>
-  <si>
-    <t>Notificación de Error "Permission denied"</t>
-  </si>
-  <si>
-    <t>CrM31</t>
-  </si>
-  <si>
-    <t>1-Se selecciona un disco sin espacio suficiente</t>
-  </si>
-  <si>
-    <t>Notifcación de Error</t>
-  </si>
-  <si>
-    <t>❓</t>
-  </si>
-  <si>
-    <t>CrM32</t>
-  </si>
-  <si>
-    <t>1-Se selecciona una carpeta válida</t>
-  </si>
-  <si>
-    <t>CrM33</t>
-  </si>
-  <si>
-    <t>Se Guarda el modelo/descripción</t>
-  </si>
-  <si>
-    <t>CrM34</t>
-  </si>
-  <si>
-    <t>Predicción del Modelo</t>
-  </si>
-  <si>
-    <t>CrM33||CrM23||CrM24</t>
-  </si>
-  <si>
-    <t>1-Se comprueba el panel "Predicción con modelo"</t>
-  </si>
-  <si>
-    <t>Panel correcto para la predicción</t>
-  </si>
-  <si>
-    <t>CrM35</t>
-  </si>
-  <si>
-    <t>1-Se comprueba que la entrada/salida son las respectivas columnas seleccionadas</t>
-  </si>
-  <si>
-    <t>Panel dividido correctamente</t>
-  </si>
-  <si>
-    <t>CrM36</t>
-  </si>
-  <si>
-    <t>1-No se escribe una entrada o se escribe un valor no numérico y se predice</t>
-  </si>
-  <si>
-    <t>Notificación de Error "Valores no numéricos"</t>
-  </si>
-  <si>
-    <t>CrM37</t>
-  </si>
-  <si>
-    <t>1-Se escribe un valor numérico en la entrada y se predice</t>
-  </si>
-  <si>
-    <t>Se predice correctamente la salida</t>
-  </si>
-  <si>
-    <t>CrM38</t>
-  </si>
-  <si>
-    <t>CrM(1||2||…..||37)</t>
-  </si>
-  <si>
-    <t>1-Se carga otro archivo</t>
-  </si>
-  <si>
-    <t>Se reinician todos los paneles</t>
-  </si>
-  <si>
-    <t>CaM0</t>
-  </si>
-  <si>
-    <t>Cargar Modelo</t>
-  </si>
-  <si>
-    <t>1-Se presiona el botón "Cargar Modelo" arriba a la izquierda</t>
-  </si>
-  <si>
-    <t>Nueva pestaña con paneles para cargar modelo</t>
-  </si>
-  <si>
-    <t>CaM1</t>
-  </si>
-  <si>
-    <t>1-Se presiona el botón"Cargar Modelo" del panel "Cargar Modelo Guardado"</t>
-  </si>
-  <si>
-    <t>Nueva ventana para selección de archivo</t>
-  </si>
-  <si>
-    <t>CaM2</t>
-  </si>
-  <si>
-    <t>1-Se exploran archivos</t>
-  </si>
-  <si>
-    <t>Solo se aceptan arhcivos Joblib</t>
-  </si>
-  <si>
-    <t>CaM3</t>
-  </si>
-  <si>
-    <t>1-Se selecciona un archivo corrupto</t>
-  </si>
-  <si>
-    <t>Notificación de Error "Error al cargar el modelo"</t>
+    <t>1-Se cambia entre pestañas "Crear Modelo" y "Cargar modelo"</t>
+  </si>
+  <si>
+    <t>CaM(0||…..12)||CrM(1…37)</t>
+  </si>
+  <si>
+    <t>No se borra el progreso en el cada pestaña</t>
+  </si>
+  <si>
+    <t>Re0</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Se hallan 3 archivos tipo MD</t>
+  </si>
+  <si>
+    <t>Re1</t>
+  </si>
+  <si>
+    <t>1-Se abre "librerías_para_GUI.md"</t>
+  </si>
+  <si>
+    <t>Se halla un documento de investigación</t>
+  </si>
+  <si>
+    <t>Re2</t>
+  </si>
+  <si>
+    <t>Research librerías</t>
+  </si>
+  <si>
+    <t>1-Se lee el documento</t>
+  </si>
+  <si>
+    <t>Se comparan y eligen librerías para la GUI en el md</t>
+  </si>
+  <si>
+    <t>Re3</t>
+  </si>
+  <si>
+    <t>1-Se abre la carpeta docs\ researches en Github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Se abre"Modelos_lineales.md" </t>
+  </si>
+  <si>
+    <t>Research Modelos lineales</t>
+  </si>
+  <si>
+    <t>Re4</t>
+  </si>
+  <si>
+    <t>Re5</t>
+  </si>
+  <si>
+    <t>Re6</t>
+  </si>
+  <si>
+    <t>Se explican correctamente los modeos lineales</t>
+  </si>
+  <si>
+    <t>Research Persistencia modelos</t>
+  </si>
+  <si>
+    <t>1-Se abre "Persistencia_modelos.md"</t>
+  </si>
+  <si>
+    <t>Se explica detalladamente la persistencia de modelos</t>
   </si>
 </sst>
 </file>
@@ -574,8 +715,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C865C549-F8D7-491B-B5A0-DEAEC76F60E7}" name="Tabla1" displayName="Tabla1" ref="D1:I46" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="D1:I46" xr:uid="{C865C549-F8D7-491B-B5A0-DEAEC76F60E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C865C549-F8D7-491B-B5A0-DEAEC76F60E7}" name="Tabla1" displayName="Tabla1" ref="D1:I41" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="D1:I41" xr:uid="{C865C549-F8D7-491B-B5A0-DEAEC76F60E7}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{89E5CABB-DA9A-41F4-819F-F69C7B220B9A}" name="ID"/>
     <tableColumn id="2" xr3:uid="{C0F89E4A-52E1-4F79-8B03-593ECF0BF318}" name="FUNCIONALIDAD"/>
@@ -585,6 +726,34 @@
     <tableColumn id="6" xr3:uid="{6423689A-066B-4266-9C96-01C7C84AA30A}" name="PASS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{44562616-F101-4E40-AFB3-1698BF3A24C3}" name="Tabla2" displayName="Tabla2" ref="D42:I55" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{7A2FBDE4-3BDB-412A-A3E0-4CDA04325ABF}" name="Columna1"/>
+    <tableColumn id="2" xr3:uid="{25E4C2E5-3CFE-4DD9-A9EA-4477808FF9A5}" name="Columna2"/>
+    <tableColumn id="3" xr3:uid="{66759CA3-E9AC-4D9F-A529-BE0AE1BB9046}" name="Columna3"/>
+    <tableColumn id="4" xr3:uid="{AF0B3DD7-3905-4953-9BFD-97C6C5703293}" name="Columna4"/>
+    <tableColumn id="5" xr3:uid="{086706AC-B641-4BDF-8EF0-668F9BD83B9B}" name="Columna5"/>
+    <tableColumn id="6" xr3:uid="{DD15FD9D-57BC-4464-94B7-BE73923BD07C}" name="Columna6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5F9A7C99-5FA9-4535-8042-A73F579A5CCA}" name="Tabla3" displayName="Tabla3" ref="D56:I62" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{9E167D48-F213-4CFD-B9AB-DC036C96D7D0}" name="Columna1"/>
+    <tableColumn id="2" xr3:uid="{E4A6527F-9BC5-495B-AEC7-65A399AA6B1E}" name="Columna2"/>
+    <tableColumn id="3" xr3:uid="{131758A9-ADDA-457B-BF2F-69851DD70256}" name="Columna3"/>
+    <tableColumn id="4" xr3:uid="{2A34D251-83BD-41E0-85CC-E96FA8186B5B}" name="Columna4"/>
+    <tableColumn id="5" xr3:uid="{E60493CF-7A5C-45FF-990C-1075FAE62ADD}" name="Columna5"/>
+    <tableColumn id="6" xr3:uid="{F2DAD690-0C1D-42C8-B011-A97A6C34BE80}" name="Columna6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -905,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480CF6BA-EE37-47B7-9844-60E33DB6B147}">
-  <dimension ref="C1:I51"/>
+  <dimension ref="C1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="118" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="118" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +1120,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>54</v>
+        <v>170</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
@@ -959,10 +1128,10 @@
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -971,7 +1140,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
         <v>9</v>
@@ -979,19 +1148,19 @@
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
         <v>9</v>
@@ -999,36 +1168,36 @@
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I6" t="s">
         <v>9</v>
@@ -1036,19 +1205,19 @@
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
         <v>25</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
       </c>
       <c r="I7" t="s">
         <v>9</v>
@@ -1056,19 +1225,19 @@
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
         <v>26</v>
       </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I8" t="s">
         <v>9</v>
@@ -1076,19 +1245,19 @@
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="I9" t="s">
         <v>9</v>
@@ -1096,19 +1265,19 @@
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" t="s">
-        <v>30</v>
       </c>
       <c r="I10" t="s">
         <v>9</v>
@@ -1116,19 +1285,19 @@
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I11" t="s">
         <v>9</v>
@@ -1136,19 +1305,19 @@
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="H12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I12" t="s">
         <v>9</v>
@@ -1156,19 +1325,19 @@
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="H13" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I13" t="s">
         <v>9</v>
@@ -1176,19 +1345,19 @@
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
         <v>42</v>
-      </c>
-      <c r="F14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" t="s">
-        <v>40</v>
       </c>
       <c r="I14" t="s">
         <v>9</v>
@@ -1196,19 +1365,19 @@
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="E15" t="s">
-        <v>43</v>
-      </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I15" t="s">
         <v>9</v>
@@ -1216,19 +1385,19 @@
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="G16" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H16" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I16" t="s">
         <v>9</v>
@@ -1236,19 +1405,19 @@
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" t="s">
         <v>53</v>
       </c>
-      <c r="G17" t="s">
-        <v>58</v>
-      </c>
       <c r="H17" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I17" t="s">
         <v>9</v>
@@ -1256,19 +1425,19 @@
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="G18" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H18" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I18" t="s">
         <v>9</v>
@@ -1276,19 +1445,19 @@
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I19" t="s">
         <v>9</v>
@@ -1296,19 +1465,19 @@
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="G20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H20" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I20" t="s">
         <v>9</v>
@@ -1316,16 +1485,16 @@
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F21" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="G21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H21" t="s">
         <v>69</v>
@@ -1336,19 +1505,19 @@
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H22" t="s">
         <v>70</v>
-      </c>
-      <c r="E22" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" t="s">
-        <v>71</v>
-      </c>
-      <c r="H22" t="s">
-        <v>72</v>
       </c>
       <c r="I22" t="s">
         <v>9</v>
@@ -1356,79 +1525,79 @@
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F23" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I23" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H24" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I24" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H25" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I25" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="G26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I26" t="s">
         <v>9</v>
@@ -1436,19 +1605,19 @@
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="F27" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="G27" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="H27" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I27" t="s">
         <v>9</v>
@@ -1456,19 +1625,19 @@
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="G28" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="H28" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I28" t="s">
         <v>9</v>
@@ -1476,19 +1645,19 @@
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="G29" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H29" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I29" t="s">
         <v>9</v>
@@ -1496,19 +1665,19 @@
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E30" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="G30" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="H30" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="I30" t="s">
         <v>9</v>
@@ -1516,19 +1685,19 @@
     </row>
     <row r="31" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="G31" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="H31" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="I31" t="s">
         <v>9</v>
@@ -1536,19 +1705,19 @@
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E32" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F32" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="G32" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="H32" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="I32" t="s">
         <v>9</v>
@@ -1556,19 +1725,19 @@
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E33" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F33" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="G33" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="H33" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="I33" t="s">
         <v>9</v>
@@ -1576,39 +1745,39 @@
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="E34" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F34" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="G34" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="H34" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="I34" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F35" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="G35" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="H35" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I35" t="s">
         <v>9</v>
@@ -1616,19 +1785,19 @@
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="E36" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F36" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="G36" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H36" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="I36" t="s">
         <v>9</v>
@@ -1636,19 +1805,19 @@
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="E37" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F37" t="s">
-        <v>119</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
+      </c>
+      <c r="G37" t="s">
+        <v>123</v>
       </c>
       <c r="H37" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I37" t="s">
         <v>9</v>
@@ -1656,19 +1825,19 @@
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="E38" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F38" t="s">
-        <v>117</v>
-      </c>
-      <c r="G38" t="s">
-        <v>123</v>
+        <v>91</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="H38" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I38" t="s">
         <v>9</v>
@@ -1676,16 +1845,16 @@
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="E39" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F39" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="G39" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H39" t="s">
         <v>127</v>
@@ -1696,19 +1865,19 @@
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="E40" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F40" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="G40" t="s">
         <v>129</v>
       </c>
       <c r="H40" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I40" t="s">
         <v>9</v>
@@ -1717,13 +1886,13 @@
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
       <c r="D41" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E41" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F41" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="G41" t="s">
         <v>133</v>
@@ -1737,19 +1906,19 @@
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E42" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F42" t="s">
         <v>6</v>
       </c>
       <c r="G42" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="H42" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I42" t="s">
         <v>9</v>
@@ -1757,19 +1926,19 @@
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E43" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F43" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G43" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="H43" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="I43" t="s">
         <v>9</v>
@@ -1777,19 +1946,19 @@
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E44" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F44" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G44" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="H44" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="I44" t="s">
         <v>9</v>
@@ -1797,32 +1966,368 @@
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" t="s">
+        <v>131</v>
+      </c>
+      <c r="F45" t="s">
+        <v>136</v>
+      </c>
+      <c r="G45" t="s">
+        <v>155</v>
+      </c>
+      <c r="H45" t="s">
+        <v>156</v>
+      </c>
+      <c r="I45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>138</v>
+      </c>
+      <c r="E46" t="s">
+        <v>131</v>
+      </c>
+      <c r="F46" t="s">
+        <v>136</v>
+      </c>
+      <c r="G46" t="s">
+        <v>157</v>
+      </c>
+      <c r="H46" t="s">
+        <v>158</v>
+      </c>
+      <c r="I46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>139</v>
+      </c>
+      <c r="E47" t="s">
+        <v>131</v>
+      </c>
+      <c r="F47" t="s">
+        <v>138</v>
+      </c>
+      <c r="G47" t="s">
+        <v>159</v>
+      </c>
+      <c r="H47" t="s">
+        <v>160</v>
+      </c>
+      <c r="I47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" t="s">
+        <v>161</v>
+      </c>
+      <c r="F48" t="s">
+        <v>139</v>
+      </c>
+      <c r="G48" t="s">
+        <v>162</v>
+      </c>
+      <c r="H48" t="s">
+        <v>163</v>
+      </c>
+      <c r="I48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>141</v>
+      </c>
+      <c r="E49" t="s">
+        <v>161</v>
+      </c>
+      <c r="F49" t="s">
+        <v>139</v>
+      </c>
+      <c r="G49" t="s">
+        <v>164</v>
+      </c>
+      <c r="H49" t="s">
+        <v>165</v>
+      </c>
+      <c r="I49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>142</v>
+      </c>
+      <c r="E50" t="s">
+        <v>161</v>
+      </c>
+      <c r="F50" t="s">
+        <v>139</v>
+      </c>
+      <c r="G50" t="s">
+        <v>123</v>
+      </c>
+      <c r="H50" t="s">
+        <v>167</v>
+      </c>
+      <c r="I50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>143</v>
+      </c>
+      <c r="E51" t="s">
+        <v>161</v>
+      </c>
+      <c r="F51" t="s">
+        <v>139</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H51" t="s">
+        <v>126</v>
+      </c>
+      <c r="I51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>144</v>
+      </c>
+      <c r="E52" t="s">
+        <v>161</v>
+      </c>
+      <c r="F52" t="s">
+        <v>139</v>
+      </c>
+      <c r="G52" t="s">
+        <v>128</v>
+      </c>
+      <c r="H52" t="s">
+        <v>127</v>
+      </c>
+      <c r="I52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
         <v>145</v>
       </c>
-      <c r="E45" t="s">
-        <v>136</v>
-      </c>
-      <c r="F45" t="s">
-        <v>142</v>
-      </c>
-      <c r="G45" t="s">
+      <c r="E53" t="s">
+        <v>161</v>
+      </c>
+      <c r="F53" t="s">
+        <v>139</v>
+      </c>
+      <c r="G53" t="s">
+        <v>129</v>
+      </c>
+      <c r="H53" t="s">
+        <v>132</v>
+      </c>
+      <c r="I53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
         <v>146</v>
       </c>
-      <c r="H45" t="s">
+      <c r="E54" t="s">
+        <v>161</v>
+      </c>
+      <c r="F54" t="s">
+        <v>169</v>
+      </c>
+      <c r="G54" t="s">
+        <v>168</v>
+      </c>
+      <c r="H54" t="s">
+        <v>134</v>
+      </c>
+      <c r="I54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
         <v>147</v>
       </c>
-      <c r="I45" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G51" s="2"/>
+      <c r="E55" t="s">
+        <v>161</v>
+      </c>
+      <c r="F55" t="s">
+        <v>172</v>
+      </c>
+      <c r="G55" t="s">
+        <v>171</v>
+      </c>
+      <c r="H55" t="s">
+        <v>173</v>
+      </c>
+      <c r="I55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>174</v>
+      </c>
+      <c r="E56" t="s">
+        <v>175</v>
+      </c>
+      <c r="G56" t="s">
+        <v>185</v>
+      </c>
+      <c r="H56" t="s">
+        <v>176</v>
+      </c>
+      <c r="I56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>177</v>
+      </c>
+      <c r="E57" t="s">
+        <v>181</v>
+      </c>
+      <c r="F57" t="s">
+        <v>174</v>
+      </c>
+      <c r="G57" t="s">
+        <v>178</v>
+      </c>
+      <c r="H57" t="s">
+        <v>179</v>
+      </c>
+      <c r="I57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>180</v>
+      </c>
+      <c r="E58" t="s">
+        <v>181</v>
+      </c>
+      <c r="F58" t="s">
+        <v>177</v>
+      </c>
+      <c r="G58" t="s">
+        <v>182</v>
+      </c>
+      <c r="H58" t="s">
+        <v>183</v>
+      </c>
+      <c r="I58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>184</v>
+      </c>
+      <c r="E59" t="s">
+        <v>187</v>
+      </c>
+      <c r="F59" t="s">
+        <v>174</v>
+      </c>
+      <c r="G59" t="s">
+        <v>186</v>
+      </c>
+      <c r="H59" t="s">
+        <v>179</v>
+      </c>
+      <c r="I59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>188</v>
+      </c>
+      <c r="E60" t="s">
+        <v>187</v>
+      </c>
+      <c r="F60" t="s">
+        <v>184</v>
+      </c>
+      <c r="G60" t="s">
+        <v>182</v>
+      </c>
+      <c r="H60" t="s">
+        <v>191</v>
+      </c>
+      <c r="I60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>189</v>
+      </c>
+      <c r="E61" t="s">
+        <v>192</v>
+      </c>
+      <c r="F61" t="s">
+        <v>174</v>
+      </c>
+      <c r="G61" t="s">
+        <v>193</v>
+      </c>
+      <c r="H61" t="s">
+        <v>179</v>
+      </c>
+      <c r="I61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>190</v>
+      </c>
+      <c r="E62" t="s">
+        <v>192</v>
+      </c>
+      <c r="F62" t="s">
+        <v>189</v>
+      </c>
+      <c r="G62" t="s">
+        <v>182</v>
+      </c>
+      <c r="H62" t="s">
+        <v>194</v>
+      </c>
+      <c r="I62" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>